<commit_message>
updated to 2019 deep space
</commit_message>
<xml_diff>
--- a/2018BeachBlitzDataAnalysis1.xlsx
+++ b/2018BeachBlitzDataAnalysis1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreyshen/PycharmProjects/DataAnalysisProgram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AD4854-1F31-CC48-A623-5D2CCAEF531C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63B8BA4-F462-AB45-965E-3B9730FEDC82}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <sheet name="7157" sheetId="36" r:id="rId36"/>
     <sheet name="7230" sheetId="37" r:id="rId37"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -284,7 +284,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +313,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -337,22 +345,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2786,10 +2797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2802,7 +2813,7 @@
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2813,7 +2824,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2835,8 +2846,26 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>3309</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>5012</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3309</v>
       </c>
@@ -2858,8 +2887,29 @@
       <c r="G3">
         <v>20.93333333333333</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>2122</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>3476</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>3309</v>
+      </c>
+      <c r="Q3">
+        <v>5012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>399</v>
       </c>
@@ -2881,8 +2931,26 @@
       <c r="G4">
         <v>18.93333333333333</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>4201</v>
+      </c>
+      <c r="K4">
+        <v>25</v>
+      </c>
+      <c r="L4">
+        <v>6072</v>
+      </c>
+      <c r="M4">
+        <v>19</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>5012</v>
       </c>
@@ -2904,8 +2972,22 @@
       <c r="G5">
         <v>18.4375</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <f>SUM(K2:K4)</f>
+        <v>36</v>
+      </c>
+      <c r="M5">
+        <f>SUM(M2:M4)</f>
+        <v>36</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>330</v>
       </c>
@@ -2927,8 +3009,26 @@
       <c r="G6">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>597</v>
+      </c>
+      <c r="K6">
+        <v>14</v>
+      </c>
+      <c r="L6">
+        <v>330</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>5124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1197</v>
       </c>
@@ -2950,8 +3050,26 @@
       <c r="G7">
         <v>18.05</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>294</v>
+      </c>
+      <c r="K7">
+        <v>22</v>
+      </c>
+      <c r="L7">
+        <v>399</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5810</v>
       </c>
@@ -2973,8 +3091,26 @@
       <c r="G8">
         <v>17.399999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>599</v>
+      </c>
+      <c r="K8">
+        <v>30</v>
+      </c>
+      <c r="L8">
+        <v>4322</v>
+      </c>
+      <c r="M8">
+        <v>20</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <v>6220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5199</v>
       </c>
@@ -2996,8 +3132,19 @@
       <c r="G9">
         <v>16.771428571428569</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <f>SUM(K6:K8)</f>
+        <v>66</v>
+      </c>
+      <c r="M9">
+        <f>SUM(M6:M8)</f>
+        <v>30</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2122</v>
       </c>
@@ -3019,8 +3166,20 @@
       <c r="G10">
         <v>16.55714285714286</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J10" s="4">
+        <v>687</v>
+      </c>
+      <c r="K10">
+        <v>11</v>
+      </c>
+      <c r="L10" s="4">
+        <v>5124</v>
+      </c>
+      <c r="M10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>687</v>
       </c>
@@ -3042,8 +3201,20 @@
       <c r="G11">
         <v>16.37142857142857</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J11" s="4">
+        <v>5199</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1197</v>
+      </c>
+      <c r="M11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>3476</v>
       </c>
@@ -3065,8 +3236,20 @@
       <c r="G12">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J12" s="4">
+        <v>2659</v>
+      </c>
+      <c r="K12">
+        <v>24</v>
+      </c>
+      <c r="L12" s="4">
+        <v>968</v>
+      </c>
+      <c r="M12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1836</v>
       </c>
@@ -3088,8 +3271,16 @@
       <c r="G13">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <f>SUM(K10:K12)</f>
+        <v>44</v>
+      </c>
+      <c r="M13">
+        <f>SUM(M10:M12)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>597</v>
       </c>
@@ -3111,8 +3302,20 @@
       <c r="G14">
         <v>14.65</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J14" s="4">
+        <v>6220</v>
+      </c>
+      <c r="K14">
+        <v>32</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1836</v>
+      </c>
+      <c r="M14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4999</v>
       </c>
@@ -3134,8 +3337,20 @@
       <c r="G15">
         <v>14.514285714285711</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J15" s="4">
+        <v>4276</v>
+      </c>
+      <c r="K15">
+        <v>18</v>
+      </c>
+      <c r="L15" s="4">
+        <v>5810</v>
+      </c>
+      <c r="M15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>696</v>
       </c>
@@ -3157,8 +3372,20 @@
       <c r="G16">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J16" s="4">
+        <v>3473</v>
+      </c>
+      <c r="K16">
+        <v>31</v>
+      </c>
+      <c r="L16" s="4">
+        <v>696</v>
+      </c>
+      <c r="M16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>5124</v>
       </c>
@@ -3180,8 +3407,16 @@
       <c r="G17">
         <v>13.266666666666669</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <f>SUM(K14:K16)</f>
+        <v>81</v>
+      </c>
+      <c r="M17">
+        <f>SUM(M14:M16)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>4276</v>
       </c>
@@ -3204,7 +3439,7 @@
         <v>11.24</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6072</v>
       </c>
@@ -3227,7 +3462,7 @@
         <v>10.71428571428571</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4322</v>
       </c>
@@ -3250,7 +3485,7 @@
         <v>10.514285714285711</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7025</v>
       </c>
@@ -3273,7 +3508,7 @@
         <v>10.375</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>294</v>
       </c>
@@ -3296,7 +3531,7 @@
         <v>10.36</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>968</v>
       </c>
@@ -3319,7 +3554,7 @@
         <v>9.8333333333333339</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2659</v>
       </c>
@@ -3342,7 +3577,7 @@
         <v>9.5500000000000007</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4201</v>
       </c>
@@ -3365,7 +3600,7 @@
         <v>9.5399999999999991</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4079</v>
       </c>
@@ -3388,7 +3623,7 @@
         <v>8.8571428571428577</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -3411,7 +3646,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2493</v>
       </c>
@@ -3434,7 +3669,7 @@
         <v>7.8166666666666664</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>7157</v>
       </c>
@@ -3457,7 +3692,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>599</v>
       </c>
@@ -3480,7 +3715,7 @@
         <v>7.3333333333333339</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3473</v>
       </c>
@@ -3503,7 +3738,7 @@
         <v>7.0750000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>6220</v>
       </c>
@@ -3645,9 +3880,23 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J10" r:id="rId1" tooltip="687" display="https://www.thebluealliance.com/team/687/2018" xr:uid="{7F90C160-FF41-AB44-B99D-AB1AE47F8BB3}"/>
+    <hyperlink ref="J11" r:id="rId2" tooltip="5199" display="https://www.thebluealliance.com/team/5199/2018" xr:uid="{6AFC0E64-0A4B-8848-B527-5FA3831996DE}"/>
+    <hyperlink ref="J12" r:id="rId3" tooltip="2659" display="https://www.thebluealliance.com/team/2659/2018" xr:uid="{4DF58EBD-689A-9C4A-80D4-D9BFB9B63F6F}"/>
+    <hyperlink ref="L10" r:id="rId4" tooltip="5124" display="https://www.thebluealliance.com/team/5124/2018" xr:uid="{550A065F-4022-E04D-BD69-F9BCC14F82C4}"/>
+    <hyperlink ref="L11" r:id="rId5" tooltip="1197" display="https://www.thebluealliance.com/team/1197/2018" xr:uid="{1BD0DB83-6B71-374E-995E-A5140B3B10DA}"/>
+    <hyperlink ref="L12" r:id="rId6" tooltip="968" display="https://www.thebluealliance.com/team/968/2018" xr:uid="{39D5D528-BF80-D248-BA55-8D4E4BB82000}"/>
+    <hyperlink ref="L14" r:id="rId7" tooltip="1836" display="https://www.thebluealliance.com/team/1836/2018" xr:uid="{9726D6A9-6F03-EA46-BDAD-025205326EA5}"/>
+    <hyperlink ref="L15" r:id="rId8" tooltip="5810" display="https://www.thebluealliance.com/team/5810/2018" xr:uid="{521C877D-E20F-5142-98C8-95ED58AE83C8}"/>
+    <hyperlink ref="L16" r:id="rId9" tooltip="696" display="https://www.thebluealliance.com/team/696/2018" xr:uid="{0333725B-0829-3345-8337-AA626D27F245}"/>
+    <hyperlink ref="J14" r:id="rId10" tooltip="6220" display="https://www.thebluealliance.com/team/6220/2018" xr:uid="{E70DC13B-4CC0-774D-8AFA-6CDDC8219C32}"/>
+    <hyperlink ref="J15" r:id="rId11" tooltip="4276" display="https://www.thebluealliance.com/team/4276/2018" xr:uid="{4479B9D4-FF13-F24C-9E53-2FF6E9DB9B0A}"/>
+    <hyperlink ref="J16" r:id="rId12" tooltip="3473" display="https://www.thebluealliance.com/team/3473/2018" xr:uid="{7B08F9A0-01EA-B94C-A00B-BF3BD3B4DCCE}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4378,41 +4627,41 @@
       <c r="A1">
         <v>10</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="2">
         <v>1197</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -4584,27 +4833,27 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">

</xml_diff>